<commit_message>
rounding for ind breakout fig
</commit_message>
<xml_diff>
--- a/data-extra/industry_piechart.xlsx
+++ b/data-extra/industry_piechart.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrownin\GitHub\LEEP\data-extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71D805B-5253-4182-9241-0274D83E1C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945E5EC2-BD43-4F68-9CD5-89846B41E510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Industry</t>
   </si>
@@ -61,15 +72,6 @@
   </si>
   <si>
     <t>Other Light Industry</t>
-  </si>
-  <si>
-    <t>Primary Metals</t>
-  </si>
-  <si>
-    <t>Nonmetallic Mineral Products</t>
-  </si>
-  <si>
-    <t>Petroleum and Coal Products</t>
   </si>
   <si>
     <t>Table</t>
@@ -117,13 +119,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -409,21 +408,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" customWidth="1"/>
-    <col min="2" max="2" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -433,312 +432,139 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2">
-        <v>8.8800000000000004E-2</v>
-      </c>
-      <c r="D2" s="4">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2">
-        <v>2.2499999999999999E-2</v>
-      </c>
-      <c r="D3" s="4">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2">
-        <v>0.2351</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2">
-        <v>0.13539999999999999</v>
-      </c>
-      <c r="D5" s="4">
-        <v>1</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2">
-        <v>0.21709999999999999</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="2">
-        <v>7.6899999999999996E-2</v>
-      </c>
-      <c r="D7" s="4">
-        <v>1</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2">
-        <v>7.6700000000000004E-2</v>
-      </c>
-      <c r="D8" s="4">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="2">
-        <v>0.14749999999999999</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0.1221</v>
-      </c>
-      <c r="D10" s="4">
-        <v>2</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="2">
-        <v>5.7500000000000002E-2</v>
-      </c>
-      <c r="D11" s="4">
-        <v>2</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0.2351</v>
-      </c>
-      <c r="D12" s="4">
-        <v>2</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="2">
-        <v>0.13539999999999999</v>
-      </c>
-      <c r="D13" s="4">
-        <v>2</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0.2258</v>
-      </c>
-      <c r="D14" s="4">
-        <v>2</v>
-      </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="2">
-        <v>7.6700000000000004E-2</v>
-      </c>
-      <c r="D15" s="4">
-        <v>2</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0.14749999999999999</v>
-      </c>
-      <c r="D16" s="4">
-        <v>2</v>
-      </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
+      <c r="C9">
+        <v>15</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>